<commit_message>
adding cout don and doc updates
</commit_message>
<xml_diff>
--- a/Docs/Work-effort.xlsx
+++ b/Docs/Work-effort.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Assessment\BidSystem\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6F8E12-B0D6-42A3-8288-48C8EC4B5444}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F24F43-7A9A-430B-A5AA-B317FE7231E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C261C90-82A8-40F7-9FB8-48658854AB8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C261C90-82A8-40F7-9FB8-48658854AB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Feature</t>
   </si>
@@ -159,24 +159,12 @@
     <t>Identify design for Notification</t>
   </si>
   <si>
-    <t>implement tests</t>
-  </si>
-  <si>
     <t>Effort(days)</t>
   </si>
   <si>
-    <t>add test projects</t>
-  </si>
-  <si>
     <t>implement  tests for endpoints</t>
   </si>
   <si>
-    <t>investigate about signalR</t>
-  </si>
-  <si>
-    <t>implement notification  model</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -240,15 +228,9 @@
     <t>Auto change  New to active at scheduled time(ADMIN)</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Notify all the applicants of selected bids</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>implement schedular to run daily and get finished bids info-serverside</t>
   </si>
   <si>
@@ -262,6 +244,21 @@
   </si>
   <si>
     <t>impelent required back end  project structure</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Investigate about signalR</t>
+  </si>
+  <si>
+    <t>Implement tests</t>
+  </si>
+  <si>
+    <t>Add test projects</t>
+  </si>
+  <si>
+    <t>Implement notification  model</t>
   </si>
 </sst>
 </file>
@@ -633,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48ECC3FA-3F31-4A45-9E41-D0D70F051B7B}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,10 +655,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -675,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -686,7 +683,7 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -697,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -713,13 +710,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -731,13 +728,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -748,7 +745,7 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -759,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -770,7 +767,7 @@
         <v>0.5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -784,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -795,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -806,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -817,7 +814,7 @@
         <v>0.5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -828,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -839,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -850,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -861,304 +858,315 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1">
         <v>1.5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1">
         <v>0.5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" s="1">
         <v>0.5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>26</v>
+      <c r="B30" t="s">
+        <v>30</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>31</v>
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="1">
         <v>0.5</v>
       </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="1">
-        <v>5</v>
-      </c>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>27</v>
-      </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D39" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>36</v>
-      </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D50" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.3">
@@ -1167,13 +1175,13 @@
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.3">
@@ -1181,78 +1189,71 @@
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>51</v>
-      </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D59" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D60" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
@@ -1263,37 +1264,37 @@
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
+      <c r="B66" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" t="s">
-        <v>38</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D69" s="1">
-        <v>1</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D70" s="1"/>
@@ -1316,105 +1317,97 @@
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
+      <c r="A75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>39</v>
-      </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>71</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="1">
+        <v>2</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D79" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D80" s="1">
         <v>2</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D81" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>54</v>
+        <v>67</v>
+      </c>
+      <c r="C82" t="s">
+        <v>65</v>
       </c>
       <c r="D82" s="1">
         <v>2</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>55</v>
+      <c r="C83" t="s">
+        <v>64</v>
       </c>
       <c r="D83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>73</v>
-      </c>
-      <c r="C84" t="s">
-        <v>71</v>
-      </c>
-      <c r="D84" s="1">
-        <v>2</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C85" t="s">
-        <v>69</v>
-      </c>
-      <c r="D85" s="1">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="D89">
-        <f>SUM(D1:D85)</f>
-        <v>64.5</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <f>SUM(D1:D83)</f>
+        <v>65.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>